<commit_message>
Minor change. Test auto commit after script change.
</commit_message>
<xml_diff>
--- a/sheet/MonsterCardData.xlsx
+++ b/sheet/MonsterCardData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D00772-444E-4770-AA7D-865D8553648B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0A777C-20C5-425E-80D9-BE391E193A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6870" yWindow="3765" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6285" yWindow="4140" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="175">
   <si>
     <t>掉宝地精</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -754,6 +754,10 @@
   </si>
   <si>
     <t>机器人，杂鱼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Defect bot</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1102,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1220,7 +1224,9 @@
       <c r="D5" s="2">
         <v>4</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>174</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="3"/>
     </row>

</xml_diff>

<commit_message>
Test hook. Using venv python instead of local python.
</commit_message>
<xml_diff>
--- a/sheet/MonsterCardData.xlsx
+++ b/sheet/MonsterCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0A777C-20C5-425E-80D9-BE391E193A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61F6058-1FBB-4825-B8DD-CC481B1E9CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6285" yWindow="4140" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1106,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1308,7 +1308,9 @@
       <c r="C9" s="1">
         <v>2</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2">
+        <v>4</v>
+      </c>
       <c r="E9" s="2" t="s">
         <v>159</v>
       </c>

</xml_diff>

<commit_message>
Add tags for new cards. Changed export script to avoid empty tags.
</commit_message>
<xml_diff>
--- a/sheet/MonsterCardData.xlsx
+++ b/sheet/MonsterCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61F6058-1FBB-4825-B8DD-CC481B1E9CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074CF34C-1661-466D-BC86-C3AEE7CBD5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6285" yWindow="4140" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="186">
   <si>
     <t>掉宝地精</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -758,6 +758,50 @@
   </si>
   <si>
     <t>Defect bot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Goo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sludge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Metal slime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normal cat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Campanion cat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mob slime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slime tower</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mahjong dragon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Greater mahjong dragon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kamikaze bot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sentinel bot</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1106,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1294,7 +1338,9 @@
       <c r="E8" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3" t="s">
+        <v>184</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="3"/>
     </row>
@@ -1314,7 +1360,9 @@
       <c r="E9" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>185</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="3"/>
     </row>
@@ -1358,8 +1406,12 @@
       <c r="E11" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="2"/>
+      <c r="F11" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:9" ht="256.5" x14ac:dyDescent="0.2">
@@ -1378,8 +1430,12 @@
       <c r="E12" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="2"/>
+      <c r="F12" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:9" ht="185.25" x14ac:dyDescent="0.2">
@@ -1446,8 +1502,12 @@
         <v>4</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="2"/>
+      <c r="F15" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="213.75" x14ac:dyDescent="0.2">
@@ -1466,8 +1526,12 @@
       <c r="E16" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="2"/>
+      <c r="F16" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:9" ht="409.5" x14ac:dyDescent="0.2">
@@ -1512,8 +1576,12 @@
       <c r="E18" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="2"/>
+      <c r="F18" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="142.5" x14ac:dyDescent="0.2">
@@ -1532,8 +1600,12 @@
       <c r="E19" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="2"/>
+      <c r="F19" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="142.5" x14ac:dyDescent="0.2">
@@ -1552,8 +1624,12 @@
       <c r="E20" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="2"/>
+      <c r="F20" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:9" ht="370.5" x14ac:dyDescent="0.2">
@@ -1849,8 +1925,12 @@
         <v>4</v>
       </c>
       <c r="E32" s="2"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="2"/>
+      <c r="F32" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="H32" s="3"/>
     </row>
     <row r="33" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
@@ -1945,8 +2025,12 @@
       <c r="E36" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="F36" s="3"/>
-      <c r="G36" s="2"/>
+      <c r="F36" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="H36" s="4"/>
     </row>
     <row r="37" spans="1:8" ht="156.75" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated script, fix export bug which bypasses deck image export..
</commit_message>
<xml_diff>
--- a/sheet/MonsterCardData.xlsx
+++ b/sheet/MonsterCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074CF34C-1661-466D-BC86-C3AEE7CBD5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FC62F9-FE92-4804-A6A5-09BD3167C0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6285" yWindow="4140" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="187">
   <si>
     <t>掉宝地精</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -802,6 +802,10 @@
   </si>
   <si>
     <t>Sentinel bot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Robot</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1150,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1271,7 +1275,9 @@
       <c r="F5" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>186</v>
+      </c>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="299.25" x14ac:dyDescent="0.2">
@@ -1294,7 +1300,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>8</v>
+        <v>186</v>
       </c>
       <c r="H6" s="3"/>
     </row>
@@ -1318,7 +1324,7 @@
         <v>119</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>8</v>
+        <v>186</v>
       </c>
       <c r="H7" s="3"/>
     </row>
@@ -1341,7 +1347,9 @@
       <c r="F8" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>186</v>
+      </c>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:9" ht="285" x14ac:dyDescent="0.2">
@@ -1363,7 +1371,9 @@
       <c r="F9" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>186</v>
+      </c>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="213.75" x14ac:dyDescent="0.2">
@@ -1386,7 +1396,7 @@
         <v>12</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H10" s="4"/>
     </row>

</xml_diff>

<commit_message>
Changed Sludge card effect.
</commit_message>
<xml_diff>
--- a/sheet/MonsterCardData.xlsx
+++ b/sheet/MonsterCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FC62F9-FE92-4804-A6A5-09BD3167C0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47C0887-8A19-47A1-95BE-8C774F527933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6285" yWindow="4140" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -737,10 +737,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>回合结束时：如果本牌①在手牌，可以选手牌中1张“史莱姆”牌送墓，然后本牌点数加1。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>普通猫</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -806,6 +802,11 @@
   </si>
   <si>
     <t>Robot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从手牌发动：替换房间区1张“史莱姆”牌，被替换的牌送墓。&lt;br&gt;
+回合结束时在房间：同列前方第1张怪物牌点数减1。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1154,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1261,22 +1262,22 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B5" t="s">
         <v>172</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
-        <v>4</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>174</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H5" s="3"/>
     </row>
@@ -1300,7 +1301,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H6" s="3"/>
     </row>
@@ -1324,7 +1325,7 @@
         <v>119</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H7" s="3"/>
     </row>
@@ -1345,10 +1346,10 @@
         <v>157</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H8" s="3"/>
     </row>
@@ -1369,10 +1370,10 @@
         <v>159</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="H9" s="3"/>
     </row>
@@ -1417,7 +1418,7 @@
         <v>135</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>11</v>
@@ -1441,7 +1442,7 @@
         <v>137</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>11</v>
@@ -1513,7 +1514,7 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>18</v>
@@ -1537,7 +1538,7 @@
         <v>146</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>18</v>
@@ -1587,14 +1588,14 @@
         <v>162</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:9" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>163</v>
       </c>
@@ -1608,10 +1609,10 @@
         <v>4</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>18</v>
@@ -1635,7 +1636,7 @@
         <v>145</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>18</v>
@@ -1923,10 +1924,10 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>169</v>
+      </c>
+      <c r="B32" t="s">
         <v>170</v>
-      </c>
-      <c r="B32" t="s">
-        <v>171</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
@@ -1936,7 +1937,7 @@
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>55</v>
@@ -2036,7 +2037,7 @@
         <v>167</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Explicitly specify Call effect timing.
</commit_message>
<xml_diff>
--- a/sheet/MonsterCardData.xlsx
+++ b/sheet/MonsterCardData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47C0887-8A19-47A1-95BE-8C774F527933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204D50FE-5580-4788-8485-722A4FFE893E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6285" yWindow="4140" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -458,10 +458,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>呼唤：墓地所有同名牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>送墓时：将主牌堆顶端2张牌送墓。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -475,15 +471,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>呼唤：墓地任意1张“不死”牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回合结束时在房间区：玩家受到1伤害，然后弃置本牌。&lt;br&gt;
-呼唤：弃牌堆所有同名牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>被弃置时：玩家受到1伤害，然后本牌送墓。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -542,10 +529,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>从房间区发动：弃置1张手牌，将本牌加入手牌。&lt;br&gt;呼唤：房间区最前方任意1张怪物牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>回合结束时在房间区：选场上1张点数小于本牌的牌送墓，然后本牌点数加1。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -554,259 +537,276 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>回合结束时：弃置本牌。&lt;br&gt;
+被弃置时：从弃牌堆选1张不同名的怪物牌，加入手牌或放在房间区任意列最前方。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>被弃置时：从主牌堆抽2张牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时在房间区：弃置战利品区第1张牌，如果战利品区没有牌，则改为弃置遭遇牌堆第1张战利品牌。&lt;br&gt;
+送墓时：获得遭遇牌弃牌堆第1张战利品牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从房间区发动：弃置1张《金币》，将本牌加入手牌。&lt;br&gt;
+从手牌发动：将本牌洗回主牌堆，然后选房间区1张怪物牌送墓。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>麻将龙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从房间区或手牌发动：选同区域另1张牌，将两张牌点数合计，然后从主牌堆选1张点数与合计点数相同的牌替换本牌，被替换的本牌和同区域被选择的那张牌送墓。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大麻将龙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交锋前：选同一行另1张牌，将两张牌点数合计，然后从主牌堆选1张点数与合计点数相同的牌替换本牌，被替换的本牌和同一行中被选择的那张牌送墓。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>龙蛋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从手牌发动：用主牌堆第1张“龙”牌替换本牌。&lt;br&gt;
+回合结束时在房间区：用主牌堆第1张“龙”牌替换本牌，被替换的本牌弃置。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交锋前，可选：弃置战利品区1张战利品牌，使本牌点数加1或减1。&lt;br&gt;
+送墓时：翻开X张牌，获得其中1张战利品牌。X为本牌点数。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>杂鱼史莱姆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>史莱姆，杂鱼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>史莱姆塔</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>金属史莱姆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>因战斗送墓时：改为弃置本牌。&lt;br&gt;
+升级结算时本牌在墓地：计算墓地牌数量时加3。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>送墓时：翻开主牌堆前3张（不足3张时翻开所有）与本牌不同名的史莱姆牌，选其中1张加入手牌，其余的放在房间区任意位置。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从房间区发动：弃置1张《卷轴》，将本牌加入手牌。&lt;br&gt;
+从手牌发动：将本牌洗回主牌堆，选房间区1张牌加入手牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从手牌发动：翻开主牌堆第1张牌，如果房间区有那张牌的同名牌，则用翻开的牌替换本牌，然后洗牌。&lt;br&gt;
+从房间区发动：翻开主牌堆第1张牌，如果玩家手牌有那张牌的同名牌，则用翻开的牌替换本牌，然后洗牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>造物</t>
+  </si>
+  <si>
+    <t>造物</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从手牌送墓或弃置时：从主牌堆抽2张牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机器人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有牌进入弃牌堆时：点数减1，然后如果本牌①在房间区，则将主牌堆第1张陷阱牌放在房间区任意位置。②在手牌，则将主牌堆第1张陷阱牌加入手牌，或将房间区1张陷阱牌送墓。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在场上时持续：复制同列后方第1行第1张牌的效果和牌名。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自爆机器人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有牌进入弃牌堆时：点数减1，然后如果本牌①在房间区，则选墓地1张“机器人”牌放在房间区任意位置。②在手牌，则选墓地1张“机器人”牌加入手牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有牌进入弃牌堆时：点数减1。&lt;br&gt;
+点数为0时：如果本牌①在房间区，则玩家受到1伤害。②在手牌，则玩家可以选场上1张牌送墓。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哨戒机器人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有牌进入弃牌堆时：点数减1。&lt;br&gt;
+回合结束时：如果本牌①在房间区，则将主牌堆第1张机器人牌放在房间区任意位置。②在手牌，则将主牌堆第1张机器人牌加入手牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黏菌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>送墓时：如果房间区有“史莱姆”牌，则选房间区1个有“史莱姆”牌的单元格，将本牌放到那个单元格中。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>软泥怪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>送墓时：选弃牌堆1张怪物牌放在房间区任意位置或加入手牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>持续：如果本牌不在所在列的最前方，则同列最前方的牌点数加1。&lt;br&gt;
+送墓时：如果同列后方一行有怪物牌，则本牌不送墓而是后退一行。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随从猫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>送墓时，可选：改为弃置本牌，然后从遭遇牌弃牌堆选1张战利品牌获得。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>送墓时，可选：翻开主牌堆顶1张牌，如果不是《九命猫》，则将本牌洗回主牌堆，然后玩家抽1张牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>普通猫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>猫，杂鱼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>故障机器人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机器人，杂鱼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Defect bot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Goo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sludge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Metal slime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normal cat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Campanion cat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mob slime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slime tower</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mahjong dragon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Greater mahjong dragon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kamikaze bot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sentinel bot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Robot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从手牌发动：替换房间区1张“史莱姆”牌，被替换的牌送墓。&lt;br&gt;
+回合结束时在房间：同列前方第1张怪物牌点数减1。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时：如果本牌①在房间区，则将主牌堆第1张“史莱姆”牌放在房间区任意位置。②在手牌，则可以横置本牌，然后将主牌堆第1张“史莱姆”牌加入手牌。&lt;br&gt;
+开战前：呼唤场上所有“史莱姆”牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>进入房间区时：将主牌堆第1张“亚人”牌放在房间区任意列最前方。&lt;br&gt;
-呼唤：房间区1张同名牌。</t>
+开战前：呼唤房间区1张同名牌。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">
 回合结束时：从主牌堆选1张《哥布林》牌放在房间区任意列最前方。&lt;br&gt;
-呼唤：房间区1张点数小于本牌的“亚人”牌。</t>
+开战前：呼唤房间区1张点数小于本牌的“亚人”牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开战前：呼唤墓地所有同名牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开战前：呼唤墓地任意1张“不死”牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时在房间区：玩家受到1伤害，然后弃置本牌。&lt;br&gt;
+开战前：呼唤弃牌堆所有同名牌。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>从房间区发动：弃置1张手牌，将本牌加入手牌。&lt;br&gt;
-呼唤：房间区所有列最前方的怪物牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回合结束时：弃置本牌。&lt;br&gt;
-被弃置时：从弃牌堆选1张不同名的怪物牌，加入手牌或放在房间区任意列最前方。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>被弃置时：从主牌堆抽2张牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回合结束时在房间区：弃置战利品区第1张牌，如果战利品区没有牌，则改为弃置遭遇牌堆第1张战利品牌。&lt;br&gt;
-送墓时：获得遭遇牌弃牌堆第1张战利品牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>从房间区发动：弃置1张《金币》，将本牌加入手牌。&lt;br&gt;
-从手牌发动：将本牌洗回主牌堆，然后选房间区1张怪物牌送墓。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>麻将龙</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>从房间区或手牌发动：选同区域另1张牌，将两张牌点数合计，然后从主牌堆选1张点数与合计点数相同的牌替换本牌，被替换的本牌和同区域被选择的那张牌送墓。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>大麻将龙</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>交锋前：选同一行另1张牌，将两张牌点数合计，然后从主牌堆选1张点数与合计点数相同的牌替换本牌，被替换的本牌和同一行中被选择的那张牌送墓。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>龙蛋</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>从手牌发动：用主牌堆第1张“龙”牌替换本牌。&lt;br&gt;
-回合结束时在房间区：用主牌堆第1张“龙”牌替换本牌，被替换的本牌弃置。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>交锋前，可选：弃置战利品区1张战利品牌，使本牌点数加1或减1。&lt;br&gt;
-送墓时：翻开X张牌，获得其中1张战利品牌。X为本牌点数。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>杂鱼史莱姆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>史莱姆，杂鱼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>史莱姆塔</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>金属史莱姆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>因战斗送墓时：改为弃置本牌。&lt;br&gt;
-升级结算时本牌在墓地：计算墓地牌数量时加3。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>送墓时：翻开主牌堆前3张（不足3张时翻开所有）与本牌不同名的史莱姆牌，选其中1张加入手牌，其余的放在房间区任意位置。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>从房间区发动：弃置1张《卷轴》，将本牌加入手牌。&lt;br&gt;
-从手牌发动：将本牌洗回主牌堆，选房间区1张牌加入手牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>从手牌发动：翻开主牌堆第1张牌，如果房间区有那张牌的同名牌，则用翻开的牌替换本牌，然后洗牌。&lt;br&gt;
-从房间区发动：翻开主牌堆第1张牌，如果玩家手牌有那张牌的同名牌，则用翻开的牌替换本牌，然后洗牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>造物</t>
-  </si>
-  <si>
-    <t>造物</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>从手牌送墓或弃置时：从主牌堆抽2张牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>机器人</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有牌进入弃牌堆时：点数减1，然后如果本牌①在房间区，则将主牌堆第1张陷阱牌放在房间区任意位置。②在手牌，则将主牌堆第1张陷阱牌加入手牌，或将房间区1张陷阱牌送墓。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在场上时持续：复制同列后方第1行第1张牌的效果和牌名。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>自爆机器人</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有牌进入弃牌堆时：点数减1，然后如果本牌①在房间区，则选墓地1张“机器人”牌放在房间区任意位置。②在手牌，则选墓地1张“机器人”牌加入手牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有牌进入弃牌堆时：点数减1。&lt;br&gt;
-点数为0时：如果本牌①在房间区，则玩家受到1伤害。②在手牌，则玩家可以选场上1张牌送墓。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>哨戒机器人</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有牌进入弃牌堆时：点数减1。&lt;br&gt;
-回合结束时：如果本牌①在房间区，则将主牌堆第1张机器人牌放在房间区任意位置。②在手牌，则将主牌堆第1张机器人牌加入手牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回合结束时：如果本牌①在房间区，则将主牌堆第1张“史莱姆”牌放在房间区任意位置。②在手牌，则可以横置本牌，然后将主牌堆第1张“史莱姆”牌加入手牌。&lt;br&gt;
-呼唤：场上所有“史莱姆”牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>黏菌</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>送墓时：如果房间区有“史莱姆”牌，则选房间区1个有“史莱姆”牌的单元格，将本牌放到那个单元格中。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>软泥怪</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>送墓时：选弃牌堆1张怪物牌放在房间区任意位置或加入手牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>持续：如果本牌不在所在列的最前方，则同列最前方的牌点数加1。&lt;br&gt;
-送墓时：如果同列后方一行有怪物牌，则本牌不送墓而是后退一行。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>随从猫</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>送墓时，可选：改为弃置本牌，然后从遭遇牌弃牌堆选1张战利品牌获得。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>送墓时，可选：翻开主牌堆顶1张牌，如果不是《九命猫》，则将本牌洗回主牌堆，然后玩家抽1张牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>普通猫</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>猫，杂鱼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>故障机器人</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>机器人，杂鱼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Defect bot</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Goo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sludge</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Metal slime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Normal cat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Campanion cat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mob slime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Slime tower</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mahjong dragon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Greater mahjong dragon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Kamikaze bot</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sentinel bot</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Robot</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>从手牌发动：替换房间区1张“史莱姆”牌，被替换的牌送墓。&lt;br&gt;
-回合结束时在房间：同列前方第1张怪物牌点数减1。</t>
+开战前：呼唤房间区所有位于列最前方的怪物牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从房间区发动：弃置1张手牌，将本牌加入手牌。&lt;br&gt;开战前：呼唤房间区最前方任意1张怪物牌。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1155,8 +1155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1195,7 +1195,7 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -1204,10 +1204,10 @@
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>8</v>
@@ -1219,7 +1219,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C3" s="1">
         <v>2</v>
@@ -1228,7 +1228,7 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>5</v>
@@ -1245,7 +1245,7 @@
         <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -1254,7 +1254,7 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="2"/>
@@ -1262,10 +1262,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -1274,10 +1274,10 @@
         <v>4</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="H5" s="3"/>
     </row>
@@ -1286,7 +1286,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -1295,13 +1295,13 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="H6" s="3"/>
     </row>
@@ -1310,7 +1310,7 @@
         <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -1319,22 +1319,22 @@
         <v>4</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:9" ht="228" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -1343,22 +1343,22 @@
         <v>4</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:9" ht="285" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -1367,19 +1367,19 @@
         <v>4</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -1391,7 +1391,7 @@
         <v>4</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>12</v>
@@ -1403,7 +1403,7 @@
     </row>
     <row r="11" spans="1:9" ht="270.75" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -1415,10 +1415,10 @@
         <v>4</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>11</v>
@@ -1427,7 +1427,7 @@
     </row>
     <row r="12" spans="1:9" ht="256.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -1439,10 +1439,10 @@
         <v>4</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>11</v>
@@ -1487,10 +1487,10 @@
         <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>11</v>
@@ -1501,10 +1501,10 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -1514,7 +1514,7 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="3" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>18</v>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="16" spans="1:9" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -1535,10 +1535,10 @@
         <v>4</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>18</v>
@@ -1559,7 +1559,7 @@
         <v>4</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>160</v>
+        <v>179</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>19</v>
@@ -1573,7 +1573,7 @@
     </row>
     <row r="18" spans="1:9" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
@@ -1585,10 +1585,10 @@
         <v>4</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>18</v>
@@ -1597,7 +1597,7 @@
     </row>
     <row r="19" spans="1:9" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
@@ -1609,10 +1609,10 @@
         <v>4</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>18</v>
@@ -1621,7 +1621,7 @@
     </row>
     <row r="20" spans="1:9" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
@@ -1633,10 +1633,10 @@
         <v>4</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>18</v>
@@ -1657,7 +1657,7 @@
         <v>4</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>23</v>
@@ -1683,7 +1683,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>27</v>
@@ -1709,10 +1709,10 @@
         <v>4</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>25</v>
@@ -1733,7 +1733,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>32</v>
@@ -1743,7 +1743,7 @@
       </c>
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:9" ht="156.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="171" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>4</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>127</v>
+        <v>180</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>34</v>
@@ -1769,7 +1769,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="213.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="228" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>4</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>128</v>
+        <v>181</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>37</v>
@@ -1807,7 +1807,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>39</v>
@@ -1833,7 +1833,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>1</v>
@@ -1860,7 +1860,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>124</v>
+        <v>186</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>44</v>
@@ -1872,7 +1872,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="156.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="171" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>4</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>129</v>
+        <v>185</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>47</v>
@@ -1910,7 +1910,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>51</v>
@@ -1924,10 +1924,10 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B32" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
@@ -1937,7 +1937,7 @@
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="3" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>55</v>
@@ -1958,7 +1958,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>56</v>
@@ -1984,10 +1984,10 @@
         <v>4</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>55</v>
@@ -2008,10 +2008,10 @@
         <v>4</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>55</v>
@@ -2022,7 +2022,7 @@
     </row>
     <row r="36" spans="1:8" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B36" t="s">
         <v>54</v>
@@ -2034,10 +2034,10 @@
         <v>4</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>55</v>
@@ -2058,7 +2058,7 @@
         <v>4</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>104</v>
+        <v>182</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>64</v>
@@ -2084,10 +2084,10 @@
         <v>4</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>108</v>
+        <v>183</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>63</v>
@@ -2108,10 +2108,10 @@
         <v>4</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>68</v>
@@ -2132,10 +2132,10 @@
         <v>4</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>63</v>
@@ -2156,7 +2156,7 @@
         <v>4</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>73</v>
@@ -2180,10 +2180,10 @@
         <v>4</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>76</v>
@@ -2204,7 +2204,7 @@
         <v>4</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>80</v>
@@ -2213,7 +2213,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>81</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>4</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>109</v>
+        <v>184</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>84</v>
@@ -2253,10 +2253,10 @@
         <v>4</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
Change some effects to add hostile/controlled by player deviation.
</commit_message>
<xml_diff>
--- a/sheet/MonsterCardData.xlsx
+++ b/sheet/MonsterCardData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E628D56-8158-4E8E-8E6A-93EF3B415910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F2FD5F-27FF-4624-B1D1-ADF661D21D6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6285" yWindow="4140" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -583,10 +583,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>有牌进入弃牌堆时：点数减1，然后如果本牌①在房间区，则将主牌堆第1张陷阱牌放在房间区任意位置。②在手牌，则将主牌堆第1张陷阱牌加入手牌，或将房间区1张陷阱牌送墓。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>在场上时持续：复制同列后方第1行第1张牌的效果和牌名。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -595,21 +591,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>有牌进入弃牌堆时：点数减1，然后如果本牌①在房间区，则选墓地1张“机器人”牌放在房间区任意位置。②在手牌，则选墓地1张“机器人”牌加入手牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有牌进入弃牌堆时：点数减1。&lt;br&gt;
-点数为0时：如果本牌①在房间区，则玩家受到1伤害。②在手牌，则玩家可以选场上1张牌送墓。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>哨戒机器人</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有牌进入弃牌堆时：点数减1。&lt;br&gt;
-回合结束时：如果本牌①在房间区，则将主牌堆第1张机器人牌放在房间区任意位置。②在手牌，则将主牌堆第1张机器人牌加入手牌。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -711,11 +693,6 @@
   <si>
     <t>从手牌发动：替换房间区1张“史莱姆”牌，被替换的牌送墓。&lt;br&gt;
 回合结束时在房间：同列前方第1张怪物牌点数减1。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回合结束时：如果本牌①在房间区，则将主牌堆第1张“史莱姆”牌放在房间区任意位置。②在手牌，则可以横置本牌，然后将主牌堆第1张“史莱姆”牌加入手牌。&lt;br&gt;
-开战前：呼唤场上所有“史莱姆”牌。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -773,6 +750,29 @@
   <si>
     <t>在场上时持续：如果本牌不在所在列的最前方，则同列最前方的牌点数加1。&lt;br&gt;
 送墓时：如果同列后方一行有怪物牌，则本牌不送墓而是后退一行。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有牌进入弃牌堆时：点数减1，然后如果本牌①与玩家敌对，则将主牌堆第1张陷阱牌放在房间区任意位置。②受玩家控制，则将主牌堆第1张陷阱牌加入手牌，或将房间区1张陷阱牌送墓。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有牌进入弃牌堆时：点数减1，然后如果本牌①与玩家敌对，则选墓地1张“机器人”牌放在房间区任意位置。②受玩家控制，则选墓地1张“机器人”牌加入手牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有牌进入弃牌堆时：点数减1。&lt;br&gt;
+点数为0时：如果本牌①与玩家敌对，则玩家受到1伤害。②受玩家控制，则玩家可以选场上1张牌送墓。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有牌进入弃牌堆时：点数减1。&lt;br&gt;
+回合结束时：如果本牌①与玩家敌对，则将主牌堆第1张机器人牌放在房间区任意位置。②受玩家控制，则将主牌堆第1张机器人牌加入手牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时：如果本牌①与玩家敌对，则将主牌堆第1张“史莱姆”牌放在房间区任意位置。②受玩家控制，则可以横置本牌，然后将主牌堆第1张“史莱姆”牌加入手牌。&lt;br&gt;
+开战前：呼唤场上所有“史莱姆”牌。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1121,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1158,10 +1158,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -1170,14 +1170,14 @@
         <v>4</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="299.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="313.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1191,17 +1191,17 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>133</v>
+        <v>174</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="242.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="256.5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -1215,19 +1215,19 @@
         <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>136</v>
+        <v>175</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>108</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="228" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="242.25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B5" t="s">
         <v>132</v>
@@ -1239,19 +1239,19 @@
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>137</v>
+        <v>176</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="285" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="299.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B6" t="s">
         <v>132</v>
@@ -1263,13 +1263,13 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>139</v>
+        <v>177</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H6" s="3"/>
     </row>
@@ -1314,7 +1314,7 @@
         <v>119</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>9</v>
@@ -1338,7 +1338,7 @@
         <v>121</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>9</v>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>16</v>
@@ -1434,7 +1434,7 @@
         <v>130</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>16</v>
@@ -1455,7 +1455,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>17</v>
@@ -1469,7 +1469,7 @@
     </row>
     <row r="15" spans="1:9" ht="156.75" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -1481,10 +1481,10 @@
         <v>4</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>16</v>
@@ -1493,7 +1493,7 @@
     </row>
     <row r="16" spans="1:9" ht="199.5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -1505,10 +1505,10 @@
         <v>4</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>16</v>
@@ -1532,7 +1532,7 @@
         <v>129</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>16</v>
@@ -1553,7 +1553,7 @@
         <v>4</v>
       </c>
       <c r="E18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>4</v>
@@ -1646,7 +1646,7 @@
         <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
@@ -1655,7 +1655,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>29</v>
@@ -1670,7 +1670,7 @@
         <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
@@ -1679,7 +1679,7 @@
         <v>4</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>31</v>
@@ -1693,10 +1693,10 @@
     </row>
     <row r="24" spans="1:9" ht="213.75" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B24" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
@@ -1705,7 +1705,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>33</v>
@@ -1720,7 +1720,7 @@
         <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C25" s="1">
         <v>2</v>
@@ -1746,7 +1746,7 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C26" s="1">
         <v>1</v>
@@ -1782,7 +1782,7 @@
         <v>4</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>40</v>
@@ -1808,7 +1808,7 @@
         <v>4</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>43</v>
@@ -1832,7 +1832,7 @@
         <v>4</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>47</v>
@@ -1846,10 +1846,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B30" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>51</v>
@@ -1880,7 +1880,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>52</v>
@@ -1906,7 +1906,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>109</v>
@@ -1930,7 +1930,7 @@
         <v>4</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>105</v>
@@ -1944,7 +1944,7 @@
     </row>
     <row r="34" spans="1:8" ht="128.25" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B34" t="s">
         <v>50</v>
@@ -1956,10 +1956,10 @@
         <v>4</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>51</v>
@@ -1980,7 +1980,7 @@
         <v>4</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>60</v>
@@ -2006,7 +2006,7 @@
         <v>4</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>110</v>
@@ -2149,7 +2149,7 @@
         <v>4</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
Add strain after movement effect instead of making it a rule. Change the effects of most trap cards which only affect their own slot. They now also affect its opposite slot.
</commit_message>
<xml_diff>
--- a/sheet/MonsterCardData.xlsx
+++ b/sheet/MonsterCardData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5EC533-5926-4994-8017-57B9AFE6ED18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5355456-F2FE-4BE6-8DF5-5430F4CDC4D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -745,22 +745,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>回合结束时：本牌点数减1，然后将本牌移动到1个相邻槽位中。这之后，消灭本牌所在槽位中所有陷阱牌，再将主牌堆第1张陷阱牌放在本牌所在槽位中。本牌点数因此降低至0时，本牌不会死亡而是弃置。&lt;br&gt;
-从手牌发动：将本牌放到房间区任意槽位。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回合结束时：本牌点数减1，然后将本牌移动到1个相邻槽位中。本牌点数因此降低至0时，使本牌所在槽位中所有其他牌点数减1，然后消灭本牌，并使玩家受到1伤害。&lt;br&gt;
-从手牌发动：将本牌放到房间区任意位置。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>回合结束时：本牌点数减1。然后将墓地第1张“机器人”牌放在本牌所在槽位中，本牌在备战区时，可以改为选墓地1张“机器人”牌放在本牌所在槽位中。本牌点数因此降低至0时，本牌不会死亡而是弃置。&lt;br&gt;
 从手牌发动：将本牌放到房间区任意位置。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>回合结束时：本牌点数减1，然后将弃牌堆第1张“机器人”牌放在本牌所在槽位中，本牌在备战区时，可以改为选弃牌堆1张“机器人”牌放在本牌所在槽位中。这之后，将本牌移动到1个相邻槽位中。本牌点数因此降低至0时，本牌不会死亡而是弃置。&lt;br&gt;
+从手牌发动：将本牌放到房间区任意位置。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时：本牌点数减1，然后将本牌移动到1个相邻槽位中并横置。这之后，消灭本牌所在槽位中所有陷阱牌，再将主牌堆第1张陷阱牌放在本牌所在槽位中。本牌点数因此降低至0时，本牌不会死亡而是弃置。&lt;br&gt;
+从手牌发动：将本牌放到房间区任意槽位。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时：本牌点数减1，然后将本牌移动到1个相邻槽位中并横置。本牌点数因此降低至0时，使本牌所在槽位中所有其他牌点数减1，然后消灭本牌，并使玩家受到1伤害。&lt;br&gt;
 从手牌发动：将本牌放到房间区任意位置。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1111,7 +1111,7 @@
   <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1183,7 +1183,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>7</v>
@@ -1207,7 +1207,7 @@
         <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>108</v>
@@ -1231,7 +1231,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>147</v>
@@ -1255,7 +1255,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>148</v>

</xml_diff>

<commit_message>
Updated slime cards and robot cards. Simplify most of their effects.
</commit_message>
<xml_diff>
--- a/sheet/MonsterCardData.xlsx
+++ b/sheet/MonsterCardData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\nanDeck\DungeonCrawlDeckMaster\sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A20AB1-940B-4214-B430-7398562B1271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553D97E7-3D41-46AE-B6B0-85B698F9B5B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5940" yWindow="3255" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="179">
   <si>
     <t>掉宝地精</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -417,10 +417,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>迷你工厂</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>烟</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -476,10 +472,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Mini factory</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Nine lives</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -539,10 +531,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>金属史莱姆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>从房间区发动：弃置1张《卷轴》，将本牌加入手牌。&lt;br&gt;
 从手牌发动：将本牌洗回主牌堆，选房间区1张牌加入手牌。</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -556,10 +544,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>哨戒机器人</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>黏菌</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -629,10 +613,6 @@
   </si>
   <si>
     <t>Kamikaze bot</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sentinel bot</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -697,15 +677,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>交锋前：弃置本牌。&lt;br&gt;
-送墓时：玩家获得1SP。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>死亡时：翻开主牌堆的“史莱姆牌”直到合计点数不小于本牌点数，然后选其中1张牌放在本牌原先所在槽位，其余的牌加入手牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Doragon</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -715,41 +686,6 @@
   </si>
   <si>
     <t>交锋前：选同区域1张牌，复制其效果和牌名。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回合结束时：本牌点数减1，然后将本牌移动1格并横置。本牌点数因此降低至0时，使本牌所在槽位中所有其他牌点数减1，然后消灭本牌，并使玩家受到1伤害。&lt;br&gt;
-从手牌发动：将本牌放到房间区任意位置。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回合结束时：如果本牌点数为1，则本牌点数加1。否则本牌点数减1，并将主牌堆第1张同名牌放在与本牌相邻的槽位中。&lt;br&gt;
-死亡时：从与本牌相邻的槽位中选1张牌，使其点数加1。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回合结束时：本牌点数减1，然后将本牌移动1格并横置。这之后，消灭本牌所在槽位中所有陷阱牌，再将主牌堆或弃牌堆第1张陷阱牌放在本牌所在槽位中。本牌点数因此降低至0时，本牌不会死亡而是弃置。&lt;br&gt;
-从手牌发动：将本牌放到房间区任意槽位。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回合结束时：本牌点数减1。然后将弃牌堆第1张“机器人”牌放在本牌所在槽位中，本牌在备战区时，可以改为选弃牌堆1张“机器人”牌放在本牌所在槽位中。本牌点数因此降低至0时，本牌不会死亡而是弃置。&lt;br&gt;
-从手牌发动：将本牌放到房间区任意位置。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回合结束时：本牌点数减1，然后将本牌移动1格并横置。这之后，将主牌堆第1张怪物牌放在本牌所在槽位中，本牌在备战区时，可以改为选主牌堆1张怪物牌放在本牌所在槽位中。本牌点数因此降低至0时，本牌不会死亡而是弃置。&lt;br&gt;
-从手牌发动：将本牌放到房间区任意位置。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>开战前：呼唤所在区域内所有“史莱姆”牌。&lt;br&gt;
-回合结束时：呼唤所在区域内另1张“史莱姆”牌。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>回合结束时：如果本牌所在槽位没有其他牌，则横置本牌，本牌在房间区时，额外使玩家受到1伤害。否则选同槽位中1张其他牌，使其点数减2。&lt;br&gt;
-复位时：将本牌移动1格或移动到对位槽位。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -764,6 +700,77 @@
   <si>
     <t>回合结束时：如果房间区有道具牌，则弃置房间区1张道具牌，然后将本牌移动到同区域内任意槽位。&lt;br&gt;
 送墓时：如果遭遇牌弃牌堆顶的牌是道具牌，可以将那张牌放在房间区的一个未被清空的行或列的遭遇牌槽位，这一效果可重复至遭遇牌弃牌堆顶不是道具牌为止。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运输无人机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Carrier drone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时：将本牌与同房间同侧至多1张牌一起移动1格。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时：移动1格，然后本牌点数减1。&lt;br&gt;
+本牌因点数为0而被消灭时：使同房间内所有其他牌点数减1。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>哨戒无人机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sentinel drone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>炮塔无人机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时：如果同房间同侧没有其他怪物牌，则将主牌堆第1张怪物牌加入本牌所在房间同侧；否则移动1格。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Turret</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时：如果同房间内有陷阱牌，则消灭同房间内所有陷阱牌；否则，将主牌堆或弃牌堆第1张陷阱牌加入本牌所在房间同侧，之后移动1格。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时：选同行列其他房间对侧的1张怪物牌，使其点数减1。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>死亡时：翻开主牌堆的“史莱姆牌”直到合计点数不小于本牌点数，然后选其中1张牌加入本牌所在房间同侧，其余的牌加入手牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时：如果本牌点数为1，则本牌点数加1。否则本牌点数减1，然后将主牌堆第1张同名牌加入与本牌相邻的房间同侧。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>回合结束时：如果本牌所在房间没有其他牌，将本牌移动1格。否则选同房间1张其他牌，使其点数减2，同房间对侧有牌时，只能选对侧的牌。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交锋前：弃置本牌。&lt;br&gt;
+送墓时：玩家获得3金币。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黄金史莱姆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开战前：呼唤场上同侧所有“史莱姆”牌。&lt;br&gt;
+回合结束时：呼唤场上同侧另1张“史莱姆”牌。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1110,10 +1117,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1152,10 +1159,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -1164,115 +1171,115 @@
         <v>4</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2">
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="D4" s="2">
-        <v>4</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D5" s="2">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C6" s="1">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2">
-        <v>4</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>170</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>122</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -1281,19 +1288,17 @@
         <v>4</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>119</v>
+        <v>172</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="4"/>
+        <v>170</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -1308,7 +1313,7 @@
         <v>117</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>163</v>
+        <v>10</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>9</v>
@@ -1317,31 +1322,31 @@
     </row>
     <row r="9" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>96</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="2">
         <v>4</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>11</v>
+        <v>156</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:9" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
@@ -1353,93 +1358,91 @@
         <v>4</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>174</v>
+        <v>96</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>103</v>
+        <v>11</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2">
+        <v>4</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2">
-        <v>4</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>119</v>
       </c>
       <c r="C12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2">
         <v>4</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>162</v>
-      </c>
+      <c r="E12" s="2"/>
       <c r="F12" s="3" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:9" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="2">
         <v>4</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>17</v>
+        <v>140</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>128</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
@@ -1451,34 +1454,36 @@
         <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>138</v>
+        <v>17</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="H14" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2">
         <v>4</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>16</v>
@@ -1487,60 +1492,58 @@
     </row>
     <row r="16" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="2">
         <v>4</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>177</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2">
         <v>4</v>
       </c>
-      <c r="E17" t="s">
-        <v>165</v>
+      <c r="E17" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="370.5" x14ac:dyDescent="0.2">
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C18" s="1">
         <v>2</v>
@@ -1548,25 +1551,25 @@
       <c r="D18" s="2">
         <v>4</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>175</v>
+      <c r="E18" t="s">
+        <v>158</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="370.5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
@@ -1575,48 +1578,50 @@
         <v>4</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>116</v>
+        <v>161</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="3" t="s">
-        <v>24</v>
+      <c r="H19" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="C20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" s="2">
         <v>4</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>104</v>
+        <v>25</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="21" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>154</v>
+        <v>20</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -1625,22 +1630,22 @@
         <v>4</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
@@ -1649,48 +1654,48 @@
         <v>4</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H22" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>158</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C23" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2">
         <v>4</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="H23" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>153</v>
       </c>
       <c r="B24" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C24" s="1">
         <v>2</v>
@@ -1699,74 +1704,72 @@
         <v>4</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H24" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C25" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" s="2">
         <v>4</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>28</v>
       </c>
       <c r="H25" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2">
+        <v>4</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="1:9" ht="384.75" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" ht="384.75" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>37</v>
-      </c>
-      <c r="B26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-      <c r="D26" s="2">
-        <v>4</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>42</v>
       </c>
       <c r="B27" t="s">
         <v>38</v>
@@ -1778,70 +1781,74 @@
         <v>4</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H27" s="4"/>
+      <c r="H27" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="28" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2">
+        <v>4</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>44</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-      <c r="D28" s="2">
-        <v>4</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="F28" s="3" t="s">
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="2">
+        <v>4</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H29" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>133</v>
-      </c>
-      <c r="B29" t="s">
-        <v>134</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2">
-        <v>4</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="30" spans="1:9" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
@@ -1849,22 +1856,18 @@
       <c r="D30" s="2">
         <v>4</v>
       </c>
-      <c r="E30" s="2" t="s">
-        <v>130</v>
-      </c>
+      <c r="E30" s="2"/>
       <c r="F30" s="3" t="s">
-        <v>52</v>
+        <v>137</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H30" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
         <v>50</v>
@@ -1876,19 +1879,21 @@
         <v>4</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>109</v>
+        <v>52</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="1:9" ht="409.5" x14ac:dyDescent="0.2">
+      <c r="H31" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32" t="s">
         <v>50</v>
@@ -1900,21 +1905,19 @@
         <v>4</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>160</v>
+        <v>128</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H32" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>131</v>
+        <v>55</v>
       </c>
       <c r="B33" t="s">
         <v>50</v>
@@ -1926,45 +1929,45 @@
         <v>4</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>142</v>
+        <v>104</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="1:8" ht="156.75" x14ac:dyDescent="0.2">
+      <c r="H33" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>127</v>
+      </c>
+      <c r="B34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="2">
+        <v>4</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8" ht="156.75" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>57</v>
-      </c>
-      <c r="B34" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1</v>
-      </c>
-      <c r="D34" s="2">
-        <v>4</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>62</v>
       </c>
       <c r="B35" t="s">
         <v>58</v>
@@ -1976,184 +1979,210 @@
         <v>4</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="H35" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="1">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2">
+        <v>4</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" t="s">
         <v>63</v>
       </c>
-      <c r="C36" s="1">
-        <v>1</v>
-      </c>
-      <c r="D36" s="2">
-        <v>4</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F36" s="3" t="s">
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="2">
+        <v>4</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38" s="2">
+        <v>4</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>65</v>
-      </c>
-      <c r="B37" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" s="1">
-        <v>1</v>
-      </c>
-      <c r="D37" s="2">
-        <v>4</v>
-      </c>
-      <c r="E37" s="2" t="s">
+      <c r="G38" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="1">
+        <v>2</v>
+      </c>
+      <c r="D39" s="2">
+        <v>4</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="1">
+        <v>1</v>
+      </c>
+      <c r="D40" s="2">
+        <v>4</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" ht="57" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="D41" s="2">
+        <v>4</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>66</v>
-      </c>
-      <c r="B38" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="1">
-        <v>2</v>
-      </c>
-      <c r="D38" s="2">
-        <v>4</v>
-      </c>
-      <c r="E38" s="2" t="s">
+      <c r="F41" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="1">
+        <v>1</v>
+      </c>
+      <c r="D42" s="2">
+        <v>4</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2">
+        <v>4</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F38" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>70</v>
-      </c>
-      <c r="B39" t="s">
-        <v>71</v>
-      </c>
-      <c r="C39" s="1">
-        <v>1</v>
-      </c>
-      <c r="D39" s="2">
-        <v>4</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="1:8" ht="57" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>73</v>
-      </c>
-      <c r="B40" t="s">
-        <v>74</v>
-      </c>
-      <c r="C40" s="1">
-        <v>1</v>
-      </c>
-      <c r="D40" s="2">
-        <v>4</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G40" s="2" t="s">
+      <c r="F43" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="142.5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" t="s">
-        <v>78</v>
-      </c>
-      <c r="C41" s="1">
-        <v>1</v>
-      </c>
-      <c r="D41" s="2">
-        <v>4</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>93</v>
-      </c>
-      <c r="B42" t="s">
-        <v>74</v>
-      </c>
-      <c r="C42" s="1">
-        <v>1</v>
-      </c>
-      <c r="D42" s="2">
-        <v>4</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H42" s="3"/>
+      <c r="H43" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>